<commit_message>
eims-toi updates per readme doc Aug 11
</commit_message>
<xml_diff>
--- a/eims-toi-transect/eims-transect.xlsx
+++ b/eims-toi-transect/eims-transect.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>attributeName</t>
   </si>
@@ -53,7 +53,49 @@
     <t>missingValueCodeExplanation</t>
   </si>
   <si>
-    <t>Date and time in UTC</t>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>dimensionless</t>
+  </si>
+  <si>
+    <t>degree</t>
+  </si>
+  <si>
+    <t>biosat</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>Missing value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent biological saturation, the oxygen-argon ratio divided by the equilibrium value of that ratio </t>
+  </si>
+  <si>
+    <t>Oxygen-argon ratio of EIMS sample from underway corrected for air values</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>Depth of sample below sea surface. URI http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
+  </si>
+  <si>
+    <t>meter</t>
+  </si>
+  <si>
+    <t>datetime_utc_matlab</t>
+  </si>
+  <si>
+    <t>O2_Ar_ratio</t>
+  </si>
+  <si>
+    <t>latitude_matlab</t>
+  </si>
+  <si>
+    <t>longitude_matlab</t>
   </si>
   <si>
     <t>Date</t>
@@ -62,61 +104,25 @@
     <t>YYYY-MM-DD hh:mm:ss</t>
   </si>
   <si>
-    <t>UTC date and time in MATLAB serial date number format</t>
-  </si>
-  <si>
-    <t>numeric</t>
-  </si>
-  <si>
-    <t>dimensionless</t>
-  </si>
-  <si>
-    <t>Latitude of sample event</t>
-  </si>
-  <si>
-    <t>degree</t>
-  </si>
-  <si>
-    <t>Longitude of sample event</t>
-  </si>
-  <si>
-    <t>biosat</t>
-  </si>
-  <si>
-    <t>NaN</t>
-  </si>
-  <si>
-    <t>Missing value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent biological saturation, the oxygen-argon ratio divided by the equilibrium value of that ratio </t>
-  </si>
-  <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>Oxygen-argon ratio of EIMS sample from underway corrected for air values</t>
-  </si>
-  <si>
-    <t>depth</t>
-  </si>
-  <si>
-    <t>Depth of sample below sea surface. URI http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
-  </si>
-  <si>
-    <t>meter</t>
-  </si>
-  <si>
-    <t>datetime_utc</t>
-  </si>
-  <si>
-    <t>datetime_utc_matlab</t>
-  </si>
-  <si>
-    <t>O2_Ar_ratio</t>
+    <t>latitude_API</t>
+  </si>
+  <si>
+    <t>longitude_API</t>
+  </si>
+  <si>
+    <t>Latitude of sample event provided by NES-LTER API</t>
+  </si>
+  <si>
+    <t>Longitude of sample event provided by NES-LTER API</t>
+  </si>
+  <si>
+    <t>Latitude of sample event provided by PI</t>
+  </si>
+  <si>
+    <t>Longitude of sample event provided by PI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI-provided UTC date and time </t>
   </si>
 </sst>
 </file>
@@ -471,15 +477,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.3984375" customWidth="1"/>
     <col min="2" max="2" width="76.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -508,112 +514,126 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
         <v>17</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>12</v>
       </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" t="s">
-        <v>18</v>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
metadata updates and handling incorrect datetimes
</commit_message>
<xml_diff>
--- a/eims-toi-transect/eims-transect.xlsx
+++ b/eims-toi-transect/eims-transect.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\eims-toi-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F324011-D97B-4CB8-A726-D4E31BE813A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580"/>
+    <workbookView xWindow="-25104" yWindow="-2916" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -71,9 +66,6 @@
     <t>Missing value</t>
   </si>
   <si>
-    <t xml:space="preserve">Percent biological saturation, the oxygen-argon ratio divided by the equilibrium value of that ratio </t>
-  </si>
-  <si>
     <t>Oxygen-argon ratio of EIMS sample from underway corrected for air values</t>
   </si>
   <si>
@@ -120,12 +112,15 @@
   </si>
   <si>
     <t>Data product depth of sample below sea surface, for underway samples depth of ship's intake. URI http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
+  </si>
+  <si>
+    <t>Percent biological saturation, [ (O2/Ar) meas / (O2/Ar)equilibrium - 1 ]*x100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -473,11 +468,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B19"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -511,35 +506,35 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -550,10 +545,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -564,16 +559,16 @@
     </row>
     <row r="6" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -581,7 +576,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -598,10 +593,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
correct toi-transect desc and biosat def
</commit_message>
<xml_diff>
--- a/eims-toi-transect/eims-transect.xlsx
+++ b/eims-toi-transect/eims-transect.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\eims-toi-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F324011-D97B-4CB8-A726-D4E31BE813A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8049DA-86B9-45CB-9653-0958A5EA062E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25104" yWindow="-2916" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
     <t>Data product depth of sample below sea surface, for underway samples depth of ship's intake. URI http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
   </si>
   <si>
-    <t>Percent biological saturation, [ (O2/Ar) meas / (O2/Ar)equilibrium - 1 ]*x100</t>
+    <t>Percent biological saturation, [ (O2/Ar) meas / (O2/Ar)equilibrium - 1 ]x100</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>